<commit_message>
Removed blank columns which were throwing errors
</commit_message>
<xml_diff>
--- a/processed_data/participants_cleaned/Babylab_WesternSydney_12-15m_bi_GF_Participant_20190107.xlsx
+++ b/processed_data/participants_cleaned/Babylab_WesternSydney_12-15m_bi_GF_Participant_20190107.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.uws.edu.au\dfshare\HomesK-W$\30044036\Desktop\WSU\Project_ManyBabies_Bil_Dhanya\ManyBabies_GazeFollowing_Coding\Final_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krista/Repos/gaze-following-analysis/processed_data/participants_cleaned/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0B6384-9E7E-F745-961C-485EE4782ECB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="165" windowWidth="10125" windowHeight="7155" tabRatio="630"/>
+    <workbookView xWindow="100" yWindow="460" windowWidth="21400" windowHeight="12800" tabRatio="630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="12-15_Bil" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -403,7 +397,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -464,7 +458,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -555,6 +549,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -590,6 +601,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -765,19 +793,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BG43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BF43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="AU8" sqref="AU8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -919,41 +947,41 @@
       <c r="AU1" t="s">
         <v>46</v>
       </c>
+      <c r="AV1" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="AW1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="BF1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="BG1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>123</v>
       </c>
@@ -1095,6 +1123,7 @@
       <c r="AU2" t="s">
         <v>74</v>
       </c>
+      <c r="AV2" s="1"/>
       <c r="AW2" s="1"/>
       <c r="AX2" s="1"/>
       <c r="AY2" s="1"/>
@@ -1105,9 +1134,8 @@
       <c r="BD2" s="1"/>
       <c r="BE2" s="1"/>
       <c r="BF2" s="1"/>
-      <c r="BG2" s="1"/>
-    </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:58" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
@@ -1247,7 +1275,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:58" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>123</v>
       </c>
@@ -1387,7 +1415,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:58" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>123</v>
       </c>
@@ -1527,7 +1555,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>123</v>
       </c>
@@ -1667,7 +1695,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:58" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>123</v>
       </c>
@@ -1807,7 +1835,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:58" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>123</v>
       </c>
@@ -1947,7 +1975,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>123</v>
       </c>
@@ -2087,7 +2115,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>123</v>
       </c>
@@ -2227,7 +2255,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:58" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>123</v>
       </c>
@@ -2367,7 +2395,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:58" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>123</v>
       </c>
@@ -2510,7 +2538,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:58" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>123</v>
       </c>
@@ -2653,7 +2681,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:58" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>123</v>
       </c>
@@ -2793,7 +2821,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:58" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>123</v>
       </c>
@@ -2933,7 +2961,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:58" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>123</v>
       </c>
@@ -3073,7 +3101,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>123</v>
       </c>
@@ -3213,7 +3241,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>123</v>
       </c>
@@ -3353,67 +3381,67 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="2"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" s="2"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B43" s="2"/>
     </row>
   </sheetData>

</xml_diff>